<commit_message>
Refactored SpecialEffects (Turn Duration, effect % added...
Customisable on monsters themselves. Added Strength Potion with Damage boost effect. Fully Working Special Effect slot.
</commit_message>
<xml_diff>
--- a/Quizzos Sheets.xlsx
+++ b/Quizzos Sheets.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="570" windowWidth="20775" windowHeight="7620"/>
+    <workbookView xWindow="270" yWindow="570" windowWidth="20775" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Stage files" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Items" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
   <si>
     <t>Level</t>
   </si>
@@ -175,6 +175,45 @@
   </si>
   <si>
     <t>Cure</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Potions</t>
+  </si>
+  <si>
+    <t>Healing effect</t>
+  </si>
+  <si>
+    <t>Minor healing potion</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Small healing potion</t>
+  </si>
+  <si>
+    <t>Normal healing potion</t>
+  </si>
+  <si>
+    <t>Stats affected</t>
+  </si>
+  <si>
+    <t>Base damage</t>
+  </si>
+  <si>
+    <t>by %</t>
+  </si>
+  <si>
+    <t>Duration (turns)</t>
+  </si>
+  <si>
+    <t>15 gems</t>
+  </si>
+  <si>
+    <t>Strength Potion</t>
   </si>
 </sst>
 </file>
@@ -303,7 +342,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -314,6 +353,9 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -623,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
@@ -5841,17 +5883,118 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ1"/>
+  <dimension ref="A1:AML4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="8.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.875" style="1" customWidth="1"/>
+    <col min="7" max="9" width="13.125" style="1" customWidth="1"/>
+    <col min="10" max="1026" width="8.125" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1">
+        <v>150</v>
+      </c>
+      <c r="C4" s="1">
+        <v>135</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CritChance/dmg added. CritChance/RegenPotion. StageCompletionReward.
</commit_message>
<xml_diff>
--- a/Quizzos Sheets.xlsx
+++ b/Quizzos Sheets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="72">
   <si>
     <t>Level</t>
   </si>
@@ -214,6 +214,24 @@
   </si>
   <si>
     <t>Strength Potion</t>
+  </si>
+  <si>
+    <t>Regeneration Potion</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Critical Hit Chance Potion</t>
+  </si>
+  <si>
+    <t>Crit Hit Chance</t>
+  </si>
+  <si>
+    <t>10 gems</t>
+  </si>
+  <si>
+    <t>12 gems</t>
   </si>
 </sst>
 </file>
@@ -5886,7 +5904,7 @@
   <dimension ref="A1:AML4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5895,7 +5913,7 @@
     <col min="2" max="2" width="12.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.875" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.125" style="1" customWidth="1"/>
     <col min="7" max="9" width="13.125" style="1" customWidth="1"/>
     <col min="10" max="1026" width="8.125" style="1" customWidth="1"/>
   </cols>
@@ -5958,7 +5976,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="K2" s="1">
         <v>51</v>
@@ -5977,6 +5995,24 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="1">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -5990,6 +6026,24 @@
       </c>
       <c r="D4" s="1">
         <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="1">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Textmesh Sprites, Level up reward, quiz timer
</commit_message>
<xml_diff>
--- a/Quizzos Sheets.xlsx
+++ b/Quizzos Sheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="570" windowWidth="20775" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="270" yWindow="570" windowWidth="20775" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="79">
   <si>
     <t>Level</t>
   </si>
@@ -232,6 +232,27 @@
   </si>
   <si>
     <t>12 gems</t>
+  </si>
+  <si>
+    <t>Cave Spider</t>
+  </si>
+  <si>
+    <t>Low-med hp, med-high dmg</t>
+  </si>
+  <si>
+    <t>Poisonous Fangs</t>
+  </si>
+  <si>
+    <t>Boss - Bandit Leader</t>
+  </si>
+  <si>
+    <t>Cave Elder</t>
+  </si>
+  <si>
+    <t>Loyal Minion</t>
+  </si>
+  <si>
+    <t>Gastropoda</t>
   </si>
 </sst>
 </file>
@@ -681,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ80"/>
+  <dimension ref="A1:AMJ125"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5293,7 +5314,7 @@
         <v>25612.549719206301</v>
       </c>
     </row>
-    <row r="78" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>15</v>
       </c>
@@ -5465,6 +5486,1136 @@
       </c>
       <c r="B80" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1">
+        <v>2</v>
+      </c>
+      <c r="E82" s="1">
+        <v>3</v>
+      </c>
+      <c r="F82" s="1">
+        <v>4</v>
+      </c>
+      <c r="G82" s="1">
+        <v>5</v>
+      </c>
+      <c r="H82" s="1">
+        <v>6</v>
+      </c>
+      <c r="I82" s="1">
+        <v>7</v>
+      </c>
+      <c r="J82" s="1">
+        <v>8</v>
+      </c>
+      <c r="K82" s="1">
+        <v>9</v>
+      </c>
+      <c r="L82" s="1">
+        <v>10</v>
+      </c>
+      <c r="M82" s="1">
+        <v>11</v>
+      </c>
+      <c r="N82" s="1">
+        <v>12</v>
+      </c>
+      <c r="O82" s="1">
+        <v>13</v>
+      </c>
+      <c r="P82" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>15</v>
+      </c>
+      <c r="R82" s="1">
+        <v>16</v>
+      </c>
+      <c r="S82" s="1">
+        <v>17</v>
+      </c>
+      <c r="T82" s="1">
+        <v>18</v>
+      </c>
+      <c r="U82" s="1">
+        <v>19</v>
+      </c>
+      <c r="V82" s="1">
+        <v>20</v>
+      </c>
+      <c r="W82" s="1">
+        <v>21</v>
+      </c>
+      <c r="X82" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y82" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z82" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA82" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB82" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC82" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD82" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE82" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF82" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG82" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH82" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI82" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ82" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK82" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL82" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM82" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN82" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO82" s="1">
+        <v>39</v>
+      </c>
+      <c r="AP82" s="1">
+        <v>40</v>
+      </c>
+      <c r="AQ82" s="1">
+        <v>41</v>
+      </c>
+      <c r="AR82" s="1">
+        <v>42</v>
+      </c>
+      <c r="AS82" s="1">
+        <v>43</v>
+      </c>
+      <c r="AT82" s="1">
+        <v>44</v>
+      </c>
+      <c r="AU82" s="1">
+        <v>45</v>
+      </c>
+      <c r="AV82" s="1">
+        <v>46</v>
+      </c>
+      <c r="AW82" s="1">
+        <v>47</v>
+      </c>
+      <c r="AX82" s="1">
+        <v>48</v>
+      </c>
+      <c r="AY82" s="1">
+        <v>49</v>
+      </c>
+      <c r="AZ82" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C83" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C84" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B87" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C87" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B88" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C88" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B89" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C89" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1</v>
+      </c>
+      <c r="D91" s="1">
+        <v>2</v>
+      </c>
+      <c r="E91" s="1">
+        <v>3</v>
+      </c>
+      <c r="F91" s="1">
+        <v>4</v>
+      </c>
+      <c r="G91" s="1">
+        <v>5</v>
+      </c>
+      <c r="H91" s="1">
+        <v>6</v>
+      </c>
+      <c r="I91" s="1">
+        <v>7</v>
+      </c>
+      <c r="J91" s="1">
+        <v>8</v>
+      </c>
+      <c r="K91" s="1">
+        <v>9</v>
+      </c>
+      <c r="L91" s="1">
+        <v>10</v>
+      </c>
+      <c r="M91" s="1">
+        <v>11</v>
+      </c>
+      <c r="N91" s="1">
+        <v>12</v>
+      </c>
+      <c r="O91" s="1">
+        <v>13</v>
+      </c>
+      <c r="P91" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q91" s="1">
+        <v>15</v>
+      </c>
+      <c r="R91" s="1">
+        <v>16</v>
+      </c>
+      <c r="S91" s="1">
+        <v>17</v>
+      </c>
+      <c r="T91" s="1">
+        <v>18</v>
+      </c>
+      <c r="U91" s="1">
+        <v>19</v>
+      </c>
+      <c r="V91" s="1">
+        <v>20</v>
+      </c>
+      <c r="W91" s="1">
+        <v>21</v>
+      </c>
+      <c r="X91" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y91" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z91" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA91" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB91" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC91" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD91" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE91" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF91" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG91" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH91" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI91" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ91" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK91" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL91" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM91" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN91" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO91" s="1">
+        <v>39</v>
+      </c>
+      <c r="AP91" s="1">
+        <v>40</v>
+      </c>
+      <c r="AQ91" s="1">
+        <v>41</v>
+      </c>
+      <c r="AR91" s="1">
+        <v>42</v>
+      </c>
+      <c r="AS91" s="1">
+        <v>43</v>
+      </c>
+      <c r="AT91" s="1">
+        <v>44</v>
+      </c>
+      <c r="AU91" s="1">
+        <v>45</v>
+      </c>
+      <c r="AV91" s="1">
+        <v>46</v>
+      </c>
+      <c r="AW91" s="1">
+        <v>47</v>
+      </c>
+      <c r="AX91" s="1">
+        <v>48</v>
+      </c>
+      <c r="AY91" s="1">
+        <v>49</v>
+      </c>
+      <c r="AZ91" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C92" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B93" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C93" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B97" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C97" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B98" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1">
+        <v>2</v>
+      </c>
+      <c r="E100" s="1">
+        <v>3</v>
+      </c>
+      <c r="F100" s="1">
+        <v>4</v>
+      </c>
+      <c r="G100" s="1">
+        <v>5</v>
+      </c>
+      <c r="H100" s="1">
+        <v>6</v>
+      </c>
+      <c r="I100" s="1">
+        <v>7</v>
+      </c>
+      <c r="J100" s="1">
+        <v>8</v>
+      </c>
+      <c r="K100" s="1">
+        <v>9</v>
+      </c>
+      <c r="L100" s="1">
+        <v>10</v>
+      </c>
+      <c r="M100" s="1">
+        <v>11</v>
+      </c>
+      <c r="N100" s="1">
+        <v>12</v>
+      </c>
+      <c r="O100" s="1">
+        <v>13</v>
+      </c>
+      <c r="P100" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q100" s="1">
+        <v>15</v>
+      </c>
+      <c r="R100" s="1">
+        <v>16</v>
+      </c>
+      <c r="S100" s="1">
+        <v>17</v>
+      </c>
+      <c r="T100" s="1">
+        <v>18</v>
+      </c>
+      <c r="U100" s="1">
+        <v>19</v>
+      </c>
+      <c r="V100" s="1">
+        <v>20</v>
+      </c>
+      <c r="W100" s="1">
+        <v>21</v>
+      </c>
+      <c r="X100" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y100" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z100" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA100" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB100" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC100" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD100" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE100" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF100" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG100" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH100" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI100" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ100" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK100" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL100" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM100" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN100" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO100" s="1">
+        <v>39</v>
+      </c>
+      <c r="AP100" s="1">
+        <v>40</v>
+      </c>
+      <c r="AQ100" s="1">
+        <v>41</v>
+      </c>
+      <c r="AR100" s="1">
+        <v>42</v>
+      </c>
+      <c r="AS100" s="1">
+        <v>43</v>
+      </c>
+      <c r="AT100" s="1">
+        <v>44</v>
+      </c>
+      <c r="AU100" s="1">
+        <v>45</v>
+      </c>
+      <c r="AV100" s="1">
+        <v>46</v>
+      </c>
+      <c r="AW100" s="1">
+        <v>47</v>
+      </c>
+      <c r="AX100" s="1">
+        <v>48</v>
+      </c>
+      <c r="AY100" s="1">
+        <v>49</v>
+      </c>
+      <c r="AZ100" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B101" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C101" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B102" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C102" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="105" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A105" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B105" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B106" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C106" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B107" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C107" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" s="1">
+        <v>1</v>
+      </c>
+      <c r="D109" s="1">
+        <v>2</v>
+      </c>
+      <c r="E109" s="1">
+        <v>3</v>
+      </c>
+      <c r="F109" s="1">
+        <v>4</v>
+      </c>
+      <c r="G109" s="1">
+        <v>5</v>
+      </c>
+      <c r="H109" s="1">
+        <v>6</v>
+      </c>
+      <c r="I109" s="1">
+        <v>7</v>
+      </c>
+      <c r="J109" s="1">
+        <v>8</v>
+      </c>
+      <c r="K109" s="1">
+        <v>9</v>
+      </c>
+      <c r="L109" s="1">
+        <v>10</v>
+      </c>
+      <c r="M109" s="1">
+        <v>11</v>
+      </c>
+      <c r="N109" s="1">
+        <v>12</v>
+      </c>
+      <c r="O109" s="1">
+        <v>13</v>
+      </c>
+      <c r="P109" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q109" s="1">
+        <v>15</v>
+      </c>
+      <c r="R109" s="1">
+        <v>16</v>
+      </c>
+      <c r="S109" s="1">
+        <v>17</v>
+      </c>
+      <c r="T109" s="1">
+        <v>18</v>
+      </c>
+      <c r="U109" s="1">
+        <v>19</v>
+      </c>
+      <c r="V109" s="1">
+        <v>20</v>
+      </c>
+      <c r="W109" s="1">
+        <v>21</v>
+      </c>
+      <c r="X109" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y109" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z109" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA109" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB109" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC109" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD109" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE109" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF109" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG109" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH109" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI109" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ109" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK109" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL109" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM109" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN109" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO109" s="1">
+        <v>39</v>
+      </c>
+      <c r="AP109" s="1">
+        <v>40</v>
+      </c>
+      <c r="AQ109" s="1">
+        <v>41</v>
+      </c>
+      <c r="AR109" s="1">
+        <v>42</v>
+      </c>
+      <c r="AS109" s="1">
+        <v>43</v>
+      </c>
+      <c r="AT109" s="1">
+        <v>44</v>
+      </c>
+      <c r="AU109" s="1">
+        <v>45</v>
+      </c>
+      <c r="AV109" s="1">
+        <v>46</v>
+      </c>
+      <c r="AW109" s="1">
+        <v>47</v>
+      </c>
+      <c r="AX109" s="1">
+        <v>48</v>
+      </c>
+      <c r="AY109" s="1">
+        <v>49</v>
+      </c>
+      <c r="AZ109" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C110" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="111" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B111" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C111" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="114" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A114" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B114" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B115" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C115" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B116" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C118" s="1">
+        <v>1</v>
+      </c>
+      <c r="D118" s="1">
+        <v>2</v>
+      </c>
+      <c r="E118" s="1">
+        <v>3</v>
+      </c>
+      <c r="F118" s="1">
+        <v>4</v>
+      </c>
+      <c r="G118" s="1">
+        <v>5</v>
+      </c>
+      <c r="H118" s="1">
+        <v>6</v>
+      </c>
+      <c r="I118" s="1">
+        <v>7</v>
+      </c>
+      <c r="J118" s="1">
+        <v>8</v>
+      </c>
+      <c r="K118" s="1">
+        <v>9</v>
+      </c>
+      <c r="L118" s="1">
+        <v>10</v>
+      </c>
+      <c r="M118" s="1">
+        <v>11</v>
+      </c>
+      <c r="N118" s="1">
+        <v>12</v>
+      </c>
+      <c r="O118" s="1">
+        <v>13</v>
+      </c>
+      <c r="P118" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q118" s="1">
+        <v>15</v>
+      </c>
+      <c r="R118" s="1">
+        <v>16</v>
+      </c>
+      <c r="S118" s="1">
+        <v>17</v>
+      </c>
+      <c r="T118" s="1">
+        <v>18</v>
+      </c>
+      <c r="U118" s="1">
+        <v>19</v>
+      </c>
+      <c r="V118" s="1">
+        <v>20</v>
+      </c>
+      <c r="W118" s="1">
+        <v>21</v>
+      </c>
+      <c r="X118" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y118" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z118" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA118" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB118" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC118" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD118" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE118" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF118" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG118" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH118" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI118" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ118" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK118" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL118" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM118" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN118" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO118" s="1">
+        <v>39</v>
+      </c>
+      <c r="AP118" s="1">
+        <v>40</v>
+      </c>
+      <c r="AQ118" s="1">
+        <v>41</v>
+      </c>
+      <c r="AR118" s="1">
+        <v>42</v>
+      </c>
+      <c r="AS118" s="1">
+        <v>43</v>
+      </c>
+      <c r="AT118" s="1">
+        <v>44</v>
+      </c>
+      <c r="AU118" s="1">
+        <v>45</v>
+      </c>
+      <c r="AV118" s="1">
+        <v>46</v>
+      </c>
+      <c r="AW118" s="1">
+        <v>47</v>
+      </c>
+      <c r="AX118" s="1">
+        <v>48</v>
+      </c>
+      <c r="AY118" s="1">
+        <v>49</v>
+      </c>
+      <c r="AZ118" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="119" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B119" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C119" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="120" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B120" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C120" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="123" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B123" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B124" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C124" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B125" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C125" s="1">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -5903,7 +7054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>